<commit_message>
update navbar on page reload
</commit_message>
<xml_diff>
--- a/Stock Item Type Listing.xlsx
+++ b/Stock Item Type Listing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp2\htdocs\Internship-Yung-Kong-Website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4771B695-AC7B-4C07-BBBA-E63078C97852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ECB2443-9353-4D7E-83B1-125F7680C921}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1473,6 +1473,948 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Count</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet!$E$3:$F$12</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="10"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Building Materials</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Bolts &amp; Fasteners</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Hand Tools</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>General &amp; Household</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Welding &amp; Machinery</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Safety &amp; Security</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Electrical Accessories</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Plumbing</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Power Tools</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Paint</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>0</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>6</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>7</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>8</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>9</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet!$G$3:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5D15-4E0E-8C60-24B722565C3D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1975785776"/>
+        <c:axId val="1975782032"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1975785776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1975782032"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1975782032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1975785776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>457931</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>27842</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>183172</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>87924</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC77F4F9-A621-EAF1-64E6-A32B51D6DD0B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1741,7 +2683,7 @@
   <dimension ref="A1:I196"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4554,5 +5496,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
before moving about to index.php
</commit_message>
<xml_diff>
--- a/Stock Item Type Listing.xlsx
+++ b/Stock Item Type Listing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp2\htdocs\Internship-Yung-Kong-Website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27C88D1-527E-4E7A-9AA7-955B1D69145B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D054383-032C-49D7-A40F-CCFF2CA1EAC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2682,8 +2682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F170" sqref="F170"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H97" sqref="H97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2938,7 +2938,7 @@
       <c r="C13" s="8">
         <v>0</v>
       </c>
-      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="1"/>
       <c r="H13" s="10"/>

</xml_diff>

<commit_message>
add all product items and change global const naming convention
</commit_message>
<xml_diff>
--- a/Stock Item Type Listing.xlsx
+++ b/Stock Item Type Listing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp2\htdocs\Internship-Yung-Kong-Website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D054383-032C-49D7-A40F-CCFF2CA1EAC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91EC934-90D3-477F-8AC6-D5F75EE498F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13935" yWindow="360" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -877,9 +877,6 @@
     <t>HOOK,C PIN,SHELF &amp; L BRACKET &amp; SIMILARTY</t>
   </si>
   <si>
-    <t>CURTAIN ACCESORIES</t>
-  </si>
-  <si>
     <t>LAZOR GENERAL TOOLS</t>
   </si>
   <si>
@@ -1244,13 +1241,16 @@
   </si>
   <si>
     <t>Count</t>
+  </si>
+  <si>
+    <t>CURTAIN ACCESSORIES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1280,6 +1280,14 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1378,7 +1386,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1458,6 +1466,24 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2682,8 +2708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H97" sqref="H97"/>
+    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E109" sqref="E109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2705,17 +2731,17 @@
         <v>195</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>195</v>
       </c>
       <c r="G2" s="29" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2723,7 +2749,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>196</v>
+        <v>220</v>
       </c>
       <c r="C3" s="8">
         <v>0</v>
@@ -2732,7 +2758,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G3" s="30">
         <f>COUNTIF(C3:C196,0)</f>
@@ -2744,7 +2770,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="C4" s="8">
         <v>0</v>
@@ -2753,7 +2779,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="G4" s="30">
         <f>COUNTIF(C3:C197,1)</f>
@@ -2765,7 +2791,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>198</v>
+        <v>227</v>
       </c>
       <c r="C5" s="8">
         <v>0</v>
@@ -2774,7 +2800,7 @@
         <v>2</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G5" s="30">
         <f>COUNTIF(C3:C197,2)</f>
@@ -2786,7 +2812,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>199</v>
+        <v>231</v>
       </c>
       <c r="C6" s="8">
         <v>0</v>
@@ -2795,7 +2821,7 @@
         <v>3</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G6" s="30">
         <f>COUNTIF(C3:C197,3)</f>
@@ -2807,7 +2833,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
       <c r="C7" s="8">
         <v>0</v>
@@ -2816,7 +2842,7 @@
         <v>4</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G7" s="30">
         <f>COUNTIF(C3:C197,4)</f>
@@ -2828,7 +2854,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="C8" s="8">
         <v>0</v>
@@ -2837,7 +2863,7 @@
         <v>5</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G8" s="30">
         <f>COUNTIF(C3:C197,5)</f>
@@ -2849,7 +2875,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="C9" s="8">
         <v>0</v>
@@ -2858,7 +2884,7 @@
         <v>6</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G9" s="30">
         <f>COUNTIF(C3:C197,6)</f>
@@ -2870,7 +2896,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C10" s="8">
         <v>0</v>
@@ -2879,7 +2905,7 @@
         <v>7</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G10" s="30">
         <f>COUNTIF(C3:C197,7)</f>
@@ -2891,7 +2917,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="C11" s="8">
         <v>0</v>
@@ -2900,7 +2926,7 @@
         <v>8</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G11" s="30">
         <f>COUNTIF(C3:C197,8)</f>
@@ -2911,8 +2937,8 @@
       <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>205</v>
+      <c r="B12" s="31" t="s">
+        <v>199</v>
       </c>
       <c r="C12" s="8">
         <v>0</v>
@@ -2921,7 +2947,7 @@
         <v>9</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="G12" s="30">
         <f>COUNTIF(C3:C198,9)</f>
@@ -2933,7 +2959,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>206</v>
+        <v>225</v>
       </c>
       <c r="C13" s="8">
         <v>0</v>
@@ -2948,7 +2974,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="C14" s="8">
         <v>0</v>
@@ -2961,7 +2987,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="C15" s="8">
         <v>0</v>
@@ -2974,7 +3000,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C16" s="8">
         <v>0</v>
@@ -2987,7 +3013,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C17" s="8">
         <v>0</v>
@@ -3001,7 +3027,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>211</v>
+        <v>235</v>
       </c>
       <c r="C18" s="8">
         <v>0</v>
@@ -3015,7 +3041,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>212</v>
+        <v>229</v>
       </c>
       <c r="C19" s="8">
         <v>0</v>
@@ -3029,7 +3055,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="C20" s="8">
         <v>0</v>
@@ -3042,7 +3068,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>214</v>
+        <v>222</v>
       </c>
       <c r="C21" s="8">
         <v>0</v>
@@ -3054,7 +3080,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="C22" s="8">
         <v>0</v>
@@ -3066,7 +3092,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>216</v>
+        <v>232</v>
       </c>
       <c r="C23" s="8">
         <v>0</v>
@@ -3078,7 +3104,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C24" s="8">
         <v>0</v>
@@ -3090,7 +3116,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>218</v>
+        <v>236</v>
       </c>
       <c r="C25" s="8">
         <v>0</v>
@@ -3104,7 +3130,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C26" s="8">
         <v>0</v>
@@ -3118,7 +3144,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>220</v>
+        <v>238</v>
       </c>
       <c r="C27" s="8">
         <v>0</v>
@@ -3132,7 +3158,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>221</v>
+        <v>234</v>
       </c>
       <c r="C28" s="8">
         <v>0</v>
@@ -3146,7 +3172,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="C29" s="8">
         <v>0</v>
@@ -3160,7 +3186,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="C30" s="8">
         <v>0</v>
@@ -3174,7 +3200,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="C31" s="8">
         <v>0</v>
@@ -3188,7 +3214,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="C32" s="8">
         <v>0</v>
@@ -3202,7 +3228,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="C33" s="8">
         <v>0</v>
@@ -3216,7 +3242,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>227</v>
+        <v>197</v>
       </c>
       <c r="C34" s="8">
         <v>0</v>
@@ -3230,7 +3256,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>228</v>
+        <v>212</v>
       </c>
       <c r="C35" s="8">
         <v>0</v>
@@ -3244,7 +3270,7 @@
         <v>34</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="C36" s="8">
         <v>0</v>
@@ -3258,7 +3284,7 @@
         <v>35</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C37" s="8">
         <v>0</v>
@@ -3272,7 +3298,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>231</v>
+        <v>205</v>
       </c>
       <c r="C38" s="8">
         <v>0</v>
@@ -3286,7 +3312,7 @@
         <v>37</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="C39" s="8">
         <v>0</v>
@@ -3314,7 +3340,7 @@
         <v>39</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>234</v>
+        <v>201</v>
       </c>
       <c r="C41" s="8">
         <v>0</v>
@@ -3327,8 +3353,8 @@
       <c r="A42" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B42" s="7" t="s">
-        <v>235</v>
+      <c r="B42" s="31" t="s">
+        <v>206</v>
       </c>
       <c r="C42" s="8">
         <v>0</v>
@@ -3342,7 +3368,7 @@
         <v>41</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>236</v>
+        <v>198</v>
       </c>
       <c r="C43" s="8">
         <v>0</v>
@@ -3355,8 +3381,8 @@
       <c r="A44" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="7" t="s">
-        <v>237</v>
+      <c r="B44" s="31" t="s">
+        <v>200</v>
       </c>
       <c r="C44" s="8">
         <v>0</v>
@@ -3369,8 +3395,8 @@
       <c r="A45" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B45" s="7" t="s">
-        <v>238</v>
+      <c r="B45" s="31" t="s">
+        <v>209</v>
       </c>
       <c r="C45" s="8">
         <v>0</v>
@@ -3384,7 +3410,7 @@
         <v>44</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>239</v>
+        <v>252</v>
       </c>
       <c r="C46" s="12">
         <v>1</v>
@@ -3412,7 +3438,7 @@
         <v>46</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C48" s="12">
         <v>1</v>
@@ -3426,7 +3452,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="C49" s="12">
         <v>1</v>
@@ -3440,7 +3466,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="C50" s="12">
         <v>1</v>
@@ -3454,7 +3480,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="C51" s="12">
         <v>1</v>
@@ -3468,7 +3494,7 @@
         <v>50</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C52" s="12">
         <v>1</v>
@@ -3482,7 +3508,7 @@
         <v>51</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C53" s="12">
         <v>1</v>
@@ -3496,7 +3522,7 @@
         <v>52</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C54" s="12">
         <v>1</v>
@@ -3510,7 +3536,7 @@
         <v>53</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="C55" s="12">
         <v>1</v>
@@ -3524,7 +3550,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="11" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C56" s="12">
         <v>1</v>
@@ -3538,7 +3564,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="11" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="C57" s="12">
         <v>1</v>
@@ -3552,7 +3578,7 @@
         <v>56</v>
       </c>
       <c r="B58" s="11" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="C58" s="12">
         <v>1</v>
@@ -3566,7 +3592,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="11" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="C59" s="12">
         <v>1</v>
@@ -3580,7 +3606,7 @@
         <v>58</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>253</v>
+        <v>264</v>
       </c>
       <c r="C60" s="14">
         <v>2</v>
@@ -3594,7 +3620,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="C61" s="14">
         <v>2</v>
@@ -3608,7 +3634,7 @@
         <v>60</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C62" s="14">
         <v>2</v>
@@ -3622,7 +3648,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="C63" s="14">
         <v>2</v>
@@ -3636,7 +3662,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="C64" s="14">
         <v>2</v>
@@ -3649,8 +3675,8 @@
       <c r="A65" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="B65" s="13" t="s">
-        <v>258</v>
+      <c r="B65" s="32" t="s">
+        <v>256</v>
       </c>
       <c r="C65" s="14">
         <v>2</v>
@@ -3664,7 +3690,7 @@
         <v>64</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C66" s="14">
         <v>2</v>
@@ -3678,7 +3704,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="C67" s="14">
         <v>2</v>
@@ -3691,8 +3717,8 @@
       <c r="A68" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="B68" s="13" t="s">
-        <v>261</v>
+      <c r="B68" s="32" t="s">
+        <v>271</v>
       </c>
       <c r="C68" s="14">
         <v>2</v>
@@ -3706,7 +3732,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="C69" s="14">
         <v>2</v>
@@ -3719,8 +3745,8 @@
       <c r="A70" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="B70" s="13" t="s">
-        <v>263</v>
+      <c r="B70" s="32" t="s">
+        <v>267</v>
       </c>
       <c r="C70" s="14">
         <v>2</v>
@@ -3734,7 +3760,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C71" s="14">
         <v>2</v>
@@ -3762,7 +3788,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="C73" s="14">
         <v>2</v>
@@ -3776,7 +3802,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="C74" s="14">
         <v>2</v>
@@ -3790,7 +3816,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="C75" s="14">
         <v>2</v>
@@ -3804,7 +3830,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C76" s="14">
         <v>2</v>
@@ -3818,7 +3844,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="C77" s="14">
         <v>2</v>
@@ -3832,7 +3858,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="C78" s="14">
         <v>2</v>
@@ -3874,7 +3900,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="C81" s="14">
         <v>2</v>
@@ -3888,7 +3914,7 @@
         <v>80</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>275</v>
+        <v>255</v>
       </c>
       <c r="C82" s="14">
         <v>2</v>
@@ -3901,8 +3927,8 @@
       <c r="A83" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="B83" s="15" t="s">
-        <v>276</v>
+      <c r="B83" s="33" t="s">
+        <v>307</v>
       </c>
       <c r="C83" s="16">
         <v>3</v>
@@ -3916,7 +3942,7 @@
         <v>82</v>
       </c>
       <c r="B84" s="15" t="s">
-        <v>277</v>
+        <v>290</v>
       </c>
       <c r="C84" s="16">
         <v>3</v>
@@ -3930,7 +3956,7 @@
         <v>83</v>
       </c>
       <c r="B85" s="15" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="C85" s="16">
         <v>3</v>
@@ -3944,7 +3970,7 @@
         <v>84</v>
       </c>
       <c r="B86" s="15" t="s">
-        <v>279</v>
+        <v>402</v>
       </c>
       <c r="C86" s="16">
         <v>3</v>
@@ -3958,7 +3984,7 @@
         <v>85</v>
       </c>
       <c r="B87" s="15" t="s">
-        <v>280</v>
+        <v>302</v>
       </c>
       <c r="C87" s="16">
         <v>3</v>
@@ -3972,7 +3998,7 @@
         <v>86</v>
       </c>
       <c r="B88" s="15" t="s">
-        <v>281</v>
+        <v>298</v>
       </c>
       <c r="C88" s="16">
         <v>3</v>
@@ -3986,7 +4012,7 @@
         <v>87</v>
       </c>
       <c r="B89" s="15" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="C89" s="16">
         <v>3</v>
@@ -4000,7 +4026,7 @@
         <v>88</v>
       </c>
       <c r="B90" s="15" t="s">
-        <v>283</v>
+        <v>296</v>
       </c>
       <c r="C90" s="16">
         <v>3</v>
@@ -4014,7 +4040,7 @@
         <v>89</v>
       </c>
       <c r="B91" s="15" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="C91" s="16">
         <v>3</v>
@@ -4028,7 +4054,7 @@
         <v>90</v>
       </c>
       <c r="B92" s="15" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C92" s="16">
         <v>3</v>
@@ -4042,7 +4068,7 @@
         <v>91</v>
       </c>
       <c r="B93" s="15" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C93" s="16">
         <v>3</v>
@@ -4056,7 +4082,7 @@
         <v>92</v>
       </c>
       <c r="B94" s="15" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C94" s="16">
         <v>3</v>
@@ -4070,7 +4096,7 @@
         <v>93</v>
       </c>
       <c r="B95" s="15" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="C95" s="16">
         <v>3</v>
@@ -4084,7 +4110,7 @@
         <v>94</v>
       </c>
       <c r="B96" s="15" t="s">
-        <v>289</v>
+        <v>303</v>
       </c>
       <c r="C96" s="16">
         <v>3</v>
@@ -4098,7 +4124,7 @@
         <v>95</v>
       </c>
       <c r="B97" s="15" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="C97" s="16">
         <v>3</v>
@@ -4112,7 +4138,7 @@
         <v>96</v>
       </c>
       <c r="B98" s="15" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C98" s="16">
         <v>3</v>
@@ -4126,7 +4152,7 @@
         <v>97</v>
       </c>
       <c r="B99" s="15" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C99" s="16">
         <v>3</v>
@@ -4139,8 +4165,8 @@
       <c r="A100" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="B100" s="15" t="s">
-        <v>293</v>
+      <c r="B100" s="33" t="s">
+        <v>280</v>
       </c>
       <c r="C100" s="16">
         <v>3</v>
@@ -4153,8 +4179,8 @@
       <c r="A101" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="B101" s="15" t="s">
-        <v>294</v>
+      <c r="B101" s="33" t="s">
+        <v>289</v>
       </c>
       <c r="C101" s="16">
         <v>3</v>
@@ -4167,8 +4193,8 @@
       <c r="A102" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="B102" s="15" t="s">
-        <v>295</v>
+      <c r="B102" s="33" t="s">
+        <v>304</v>
       </c>
       <c r="C102" s="16">
         <v>3</v>
@@ -4181,8 +4207,8 @@
       <c r="A103" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="B103" s="15" t="s">
-        <v>296</v>
+      <c r="B103" s="33" t="s">
+        <v>306</v>
       </c>
       <c r="C103" s="16">
         <v>3</v>
@@ -4196,7 +4222,7 @@
         <v>102</v>
       </c>
       <c r="B104" s="15" t="s">
-        <v>297</v>
+        <v>291</v>
       </c>
       <c r="C104" s="16">
         <v>3</v>
@@ -4210,7 +4236,7 @@
         <v>103</v>
       </c>
       <c r="B105" s="15" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="C105" s="16">
         <v>3</v>
@@ -4224,7 +4250,7 @@
         <v>104</v>
       </c>
       <c r="B106" s="15" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="C106" s="16">
         <v>3</v>
@@ -4238,7 +4264,7 @@
         <v>105</v>
       </c>
       <c r="B107" s="15" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C107" s="16">
         <v>3</v>
@@ -4252,7 +4278,7 @@
         <v>106</v>
       </c>
       <c r="B108" s="15" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C108" s="16">
         <v>3</v>
@@ -4266,7 +4292,7 @@
         <v>107</v>
       </c>
       <c r="B109" s="15" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="C109" s="16">
         <v>3</v>
@@ -4280,7 +4306,7 @@
         <v>108</v>
       </c>
       <c r="B110" s="15" t="s">
-        <v>303</v>
+        <v>278</v>
       </c>
       <c r="C110" s="16">
         <v>3</v>
@@ -4293,8 +4319,8 @@
       <c r="A111" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="B111" s="15" t="s">
-        <v>304</v>
+      <c r="B111" s="33" t="s">
+        <v>305</v>
       </c>
       <c r="C111" s="16">
         <v>3</v>
@@ -4308,7 +4334,7 @@
         <v>110</v>
       </c>
       <c r="B112" s="15" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C112" s="16">
         <v>3</v>
@@ -4322,7 +4348,7 @@
         <v>111</v>
       </c>
       <c r="B113" s="15" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="C113" s="16">
         <v>3</v>
@@ -4336,7 +4362,7 @@
         <v>112</v>
       </c>
       <c r="B114" s="15" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="C114" s="16">
         <v>3</v>
@@ -4349,8 +4375,8 @@
       <c r="A115" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="B115" s="15" t="s">
-        <v>308</v>
+      <c r="B115" s="33" t="s">
+        <v>281</v>
       </c>
       <c r="C115" s="16">
         <v>3</v>
@@ -4364,7 +4390,7 @@
         <v>114</v>
       </c>
       <c r="B116" s="17" t="s">
-        <v>309</v>
+        <v>315</v>
       </c>
       <c r="C116" s="18">
         <v>4</v>
@@ -4378,7 +4404,7 @@
         <v>115</v>
       </c>
       <c r="B117" s="17" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C117" s="18">
         <v>4</v>
@@ -4392,7 +4418,7 @@
         <v>116</v>
       </c>
       <c r="B118" s="17" t="s">
-        <v>311</v>
+        <v>321</v>
       </c>
       <c r="C118" s="18">
         <v>4</v>
@@ -4406,7 +4432,7 @@
         <v>117</v>
       </c>
       <c r="B119" s="17" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="C119" s="18">
         <v>4</v>
@@ -4420,7 +4446,7 @@
         <v>118</v>
       </c>
       <c r="B120" s="17" t="s">
-        <v>313</v>
+        <v>319</v>
       </c>
       <c r="C120" s="18">
         <v>4</v>
@@ -4434,7 +4460,7 @@
         <v>119</v>
       </c>
       <c r="B121" s="17" t="s">
-        <v>314</v>
+        <v>322</v>
       </c>
       <c r="C121" s="18">
         <v>4</v>
@@ -4448,7 +4474,7 @@
         <v>120</v>
       </c>
       <c r="B122" s="17" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="C122" s="18">
         <v>4</v>
@@ -4461,8 +4487,8 @@
       <c r="A123" s="17" t="s">
         <v>121</v>
       </c>
-      <c r="B123" s="17" t="s">
-        <v>316</v>
+      <c r="B123" s="34" t="s">
+        <v>308</v>
       </c>
       <c r="C123" s="18">
         <v>4</v>
@@ -4476,7 +4502,7 @@
         <v>122</v>
       </c>
       <c r="B124" s="17" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="C124" s="18">
         <v>4</v>
@@ -4490,7 +4516,7 @@
         <v>123</v>
       </c>
       <c r="B125" s="17" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="C125" s="18">
         <v>4</v>
@@ -4504,7 +4530,7 @@
         <v>124</v>
       </c>
       <c r="B126" s="17" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C126" s="18">
         <v>4</v>
@@ -4518,7 +4544,7 @@
         <v>125</v>
       </c>
       <c r="B127" s="17" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="C127" s="18">
         <v>4</v>
@@ -4532,7 +4558,7 @@
         <v>126</v>
       </c>
       <c r="B128" s="17" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C128" s="18">
         <v>4</v>
@@ -4546,7 +4572,7 @@
         <v>127</v>
       </c>
       <c r="B129" s="17" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
       <c r="C129" s="18">
         <v>4</v>
@@ -4560,7 +4586,7 @@
         <v>128</v>
       </c>
       <c r="B130" s="17" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="C130" s="18">
         <v>4</v>
@@ -4574,7 +4600,7 @@
         <v>129</v>
       </c>
       <c r="B131" s="17" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="C131" s="18">
         <v>4</v>
@@ -4588,7 +4614,7 @@
         <v>130</v>
       </c>
       <c r="B132" s="19" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C132" s="20">
         <v>5</v>
@@ -4602,7 +4628,7 @@
         <v>131</v>
       </c>
       <c r="B133" s="19" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C133" s="20">
         <v>5</v>
@@ -4616,7 +4642,7 @@
         <v>132</v>
       </c>
       <c r="B134" s="19" t="s">
-        <v>327</v>
+        <v>332</v>
       </c>
       <c r="C134" s="20">
         <v>5</v>
@@ -4630,7 +4656,7 @@
         <v>133</v>
       </c>
       <c r="B135" s="19" t="s">
-        <v>328</v>
+        <v>333</v>
       </c>
       <c r="C135" s="20">
         <v>5</v>
@@ -4643,8 +4669,8 @@
       <c r="A136" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="B136" s="19" t="s">
-        <v>329</v>
+      <c r="B136" s="35" t="s">
+        <v>327</v>
       </c>
       <c r="C136" s="20">
         <v>5</v>
@@ -4657,8 +4683,8 @@
       <c r="A137" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="B137" s="19" t="s">
-        <v>330</v>
+      <c r="B137" s="35" t="s">
+        <v>334</v>
       </c>
       <c r="C137" s="20">
         <v>5</v>
@@ -4672,7 +4698,7 @@
         <v>136</v>
       </c>
       <c r="B138" s="19" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="C138" s="20">
         <v>5</v>
@@ -4686,7 +4712,7 @@
         <v>137</v>
       </c>
       <c r="B139" s="19" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="C139" s="20">
         <v>5</v>
@@ -4700,7 +4726,7 @@
         <v>138</v>
       </c>
       <c r="B140" s="19" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="C140" s="20">
         <v>5</v>
@@ -4714,7 +4740,7 @@
         <v>139</v>
       </c>
       <c r="B141" s="19" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="C141" s="20">
         <v>5</v>
@@ -4728,7 +4754,7 @@
         <v>140</v>
       </c>
       <c r="B142" s="19" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C142" s="20">
         <v>5</v>
@@ -4742,7 +4768,7 @@
         <v>141</v>
       </c>
       <c r="B143" s="19" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C143" s="20">
         <v>5</v>
@@ -4756,7 +4782,7 @@
         <v>142</v>
       </c>
       <c r="B144" s="19" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="C144" s="20">
         <v>5</v>
@@ -4770,7 +4796,7 @@
         <v>143</v>
       </c>
       <c r="B145" s="19" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="C145" s="20">
         <v>5</v>
@@ -4784,7 +4810,7 @@
         <v>144</v>
       </c>
       <c r="B146" s="21" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C146" s="22">
         <v>6</v>
@@ -4812,7 +4838,7 @@
         <v>146</v>
       </c>
       <c r="B148" s="21" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="C148" s="22">
         <v>6</v>
@@ -4826,7 +4852,7 @@
         <v>147</v>
       </c>
       <c r="B149" s="21" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="C149" s="22">
         <v>6</v>
@@ -4840,7 +4866,7 @@
         <v>148</v>
       </c>
       <c r="B150" s="21" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C150" s="22">
         <v>6</v>
@@ -4854,7 +4880,7 @@
         <v>149</v>
       </c>
       <c r="B151" s="21" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C151" s="22">
         <v>6</v>
@@ -4868,7 +4894,7 @@
         <v>150</v>
       </c>
       <c r="B152" s="21" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="C152" s="22">
         <v>6</v>
@@ -4882,7 +4908,7 @@
         <v>151</v>
       </c>
       <c r="B153" s="21" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C153" s="22">
         <v>6</v>
@@ -4896,7 +4922,7 @@
         <v>152</v>
       </c>
       <c r="B154" s="21" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="C154" s="22">
         <v>6</v>
@@ -4910,7 +4936,7 @@
         <v>153</v>
       </c>
       <c r="B155" s="21" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="C155" s="22">
         <v>6</v>
@@ -4924,7 +4950,7 @@
         <v>154</v>
       </c>
       <c r="B156" s="23" t="s">
-        <v>349</v>
+        <v>358</v>
       </c>
       <c r="C156" s="24">
         <v>7</v>
@@ -4938,7 +4964,7 @@
         <v>155</v>
       </c>
       <c r="B157" s="23" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="C157" s="24">
         <v>7</v>
@@ -4952,7 +4978,7 @@
         <v>156</v>
       </c>
       <c r="B158" s="23" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="C158" s="24">
         <v>7</v>
@@ -4965,8 +4991,8 @@
       <c r="A159" s="23" t="s">
         <v>157</v>
       </c>
-      <c r="B159" s="23" t="s">
-        <v>352</v>
+      <c r="B159" s="36" t="s">
+        <v>357</v>
       </c>
       <c r="C159" s="24">
         <v>7</v>
@@ -5008,7 +5034,7 @@
         <v>160</v>
       </c>
       <c r="B162" s="23" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C162" s="24">
         <v>7</v>
@@ -5022,7 +5048,7 @@
         <v>161</v>
       </c>
       <c r="B163" s="23" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="C163" s="24">
         <v>7</v>
@@ -5036,7 +5062,7 @@
         <v>162</v>
       </c>
       <c r="B164" s="23" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="C164" s="24">
         <v>7</v>
@@ -5050,7 +5076,7 @@
         <v>163</v>
       </c>
       <c r="B165" s="23" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="C165" s="24">
         <v>7</v>
@@ -5064,7 +5090,7 @@
         <v>164</v>
       </c>
       <c r="B166" s="23" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C166" s="24">
         <v>7</v>
@@ -5078,7 +5104,7 @@
         <v>165</v>
       </c>
       <c r="B167" s="23" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C167" s="24">
         <v>7</v>
@@ -5092,7 +5118,7 @@
         <v>166</v>
       </c>
       <c r="B168" s="23" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="C168" s="24">
         <v>7</v>
@@ -5106,7 +5132,7 @@
         <v>167</v>
       </c>
       <c r="B169" s="23" t="s">
-        <v>362</v>
+        <v>349</v>
       </c>
       <c r="C169" s="24">
         <v>7</v>
@@ -5120,7 +5146,7 @@
         <v>168</v>
       </c>
       <c r="B170" s="23" t="s">
-        <v>363</v>
+        <v>348</v>
       </c>
       <c r="C170" s="24">
         <v>7</v>
@@ -5134,7 +5160,7 @@
         <v>169</v>
       </c>
       <c r="B171" s="25" t="s">
-        <v>364</v>
+        <v>372</v>
       </c>
       <c r="C171" s="26">
         <v>8</v>
@@ -5148,7 +5174,7 @@
         <v>170</v>
       </c>
       <c r="B172" s="25" t="s">
-        <v>365</v>
+        <v>371</v>
       </c>
       <c r="C172" s="26">
         <v>8</v>
@@ -5162,7 +5188,7 @@
         <v>171</v>
       </c>
       <c r="B173" s="25" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="C173" s="26">
         <v>8</v>
@@ -5176,7 +5202,7 @@
         <v>172</v>
       </c>
       <c r="B174" s="25" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C174" s="26">
         <v>8</v>
@@ -5190,7 +5216,7 @@
         <v>173</v>
       </c>
       <c r="B175" s="25" t="s">
-        <v>368</v>
+        <v>374</v>
       </c>
       <c r="C175" s="26">
         <v>8</v>
@@ -5204,7 +5230,7 @@
         <v>174</v>
       </c>
       <c r="B176" s="25" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="C176" s="26">
         <v>8</v>
@@ -5218,7 +5244,7 @@
         <v>175</v>
       </c>
       <c r="B177" s="25" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="C177" s="26">
         <v>8</v>
@@ -5232,7 +5258,7 @@
         <v>176</v>
       </c>
       <c r="B178" s="25" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="C178" s="26">
         <v>8</v>
@@ -5246,7 +5272,7 @@
         <v>177</v>
       </c>
       <c r="B179" s="25" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="C179" s="26">
         <v>8</v>
@@ -5260,7 +5286,7 @@
         <v>178</v>
       </c>
       <c r="B180" s="25" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="C180" s="26">
         <v>8</v>
@@ -5274,7 +5300,7 @@
         <v>179</v>
       </c>
       <c r="B181" s="25" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="C181" s="26">
         <v>8</v>
@@ -5288,7 +5314,7 @@
         <v>180</v>
       </c>
       <c r="B182" s="25" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="C182" s="26">
         <v>8</v>
@@ -5302,7 +5328,7 @@
         <v>181</v>
       </c>
       <c r="B183" s="25" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="C183" s="26">
         <v>8</v>
@@ -5316,7 +5342,7 @@
         <v>182</v>
       </c>
       <c r="B184" s="25" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="C184" s="26">
         <v>8</v>
@@ -5330,7 +5356,7 @@
         <v>183</v>
       </c>
       <c r="B185" s="25" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="C185" s="26">
         <v>8</v>
@@ -5344,7 +5370,7 @@
         <v>184</v>
       </c>
       <c r="B186" s="25" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="C186" s="26">
         <v>8</v>
@@ -5358,7 +5384,7 @@
         <v>185</v>
       </c>
       <c r="B187" s="25" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C187" s="26">
         <v>8</v>
@@ -5372,7 +5398,7 @@
         <v>186</v>
       </c>
       <c r="B188" s="25" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C188" s="26">
         <v>8</v>
@@ -5386,7 +5412,7 @@
         <v>187</v>
       </c>
       <c r="B189" s="25" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="C189" s="26">
         <v>8</v>
@@ -5400,7 +5426,7 @@
         <v>188</v>
       </c>
       <c r="B190" s="25" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C190" s="26">
         <v>8</v>
@@ -5414,7 +5440,7 @@
         <v>189</v>
       </c>
       <c r="B191" s="25" t="s">
-        <v>384</v>
+        <v>364</v>
       </c>
       <c r="C191" s="26">
         <v>8</v>
@@ -5428,7 +5454,7 @@
         <v>190</v>
       </c>
       <c r="B192" s="27" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="C192" s="28">
         <v>9</v>
@@ -5442,7 +5468,7 @@
         <v>191</v>
       </c>
       <c r="B193" s="27" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C193" s="28">
         <v>9</v>
@@ -5456,7 +5482,7 @@
         <v>192</v>
       </c>
       <c r="B194" s="27" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C194" s="28">
         <v>9</v>
@@ -5470,7 +5496,7 @@
         <v>193</v>
       </c>
       <c r="B195" s="27" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="C195" s="28">
         <v>9</v>
@@ -5484,7 +5510,7 @@
         <v>194</v>
       </c>
       <c r="B196" s="27" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C196" s="28">
         <v>9</v>
@@ -5494,6 +5520,9 @@
       <c r="G196" s="1"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B146:B155">
+    <sortCondition ref="B146:B155"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
before update product to a-z
</commit_message>
<xml_diff>
--- a/Stock Item Type Listing.xlsx
+++ b/Stock Item Type Listing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp2\htdocs\Internship-Yung-Kong-Website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91EC934-90D3-477F-8AC6-D5F75EE498F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3C0BA0-1382-41D4-8ADA-B301118515AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13935" yWindow="360" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="360" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -2708,8 +2708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E109" sqref="E109"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update welding machine products, todo(product detail page)
</commit_message>
<xml_diff>
--- a/Stock Item Type Listing.xlsx
+++ b/Stock Item Type Listing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp2\htdocs\Internship-Yung-Kong-Website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BA015F0-07D5-45EA-B374-0E5BE41AA0A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C624DD62-E8FF-4CBC-B266-BFB9F6D1997C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Before" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">After!$A$2:$C$196</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">After!$A$2:$C$200</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1215" uniqueCount="418">
   <si>
     <t>Item Group</t>
   </si>
@@ -1269,13 +1269,34 @@
   </si>
   <si>
     <t>CENTRIFUGAL PUMP</t>
+  </si>
+  <si>
+    <t>30-2</t>
+  </si>
+  <si>
+    <t>31-2</t>
+  </si>
+  <si>
+    <t>49-3</t>
+  </si>
+  <si>
+    <t>49-4</t>
+  </si>
+  <si>
+    <t>49-5</t>
+  </si>
+  <si>
+    <t>49-6</t>
+  </si>
+  <si>
+    <t>49-7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1313,6 +1334,11 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1411,7 +1437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1509,6 +1535,7 @@
     <xf numFmtId="49" fontId="5" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1689,10 +1716,10 @@
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>14</c:v>
@@ -2045,10 +2072,10 @@
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>14</c:v>
@@ -3675,10 +3702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R196"/>
+  <dimension ref="A1:R200"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3744,7 +3771,7 @@
         <v>391</v>
       </c>
       <c r="G3" s="30">
-        <f>COUNTIF(C3:C196,0)</f>
+        <f>COUNTIF(C3:C200,0)</f>
         <v>43</v>
       </c>
       <c r="P3" s="7" t="s">
@@ -3774,7 +3801,7 @@
         <v>400</v>
       </c>
       <c r="G4" s="30">
-        <f>COUNTIF(C3:C197,1)</f>
+        <f>COUNTIF(C3:C200,1)</f>
         <v>14</v>
       </c>
       <c r="P4" s="7" t="s">
@@ -3804,7 +3831,7 @@
         <v>392</v>
       </c>
       <c r="G5" s="30">
-        <f>COUNTIF(C3:C197,2)</f>
+        <f>COUNTIF(C3:C200,2)</f>
         <v>23</v>
       </c>
       <c r="P5" s="7" t="s">
@@ -3834,8 +3861,8 @@
         <v>393</v>
       </c>
       <c r="G6" s="30">
-        <f>COUNTIF(C3:C197,3)</f>
-        <v>33</v>
+        <f>COUNTIF(C3:C200,3)</f>
+        <v>43</v>
       </c>
       <c r="P6" s="7" t="s">
         <v>4</v>
@@ -3864,8 +3891,8 @@
         <v>394</v>
       </c>
       <c r="G7" s="30">
-        <f>COUNTIF(C3:C197,4)</f>
-        <v>16</v>
+        <f>COUNTIF(C3:C200,4)</f>
+        <v>10</v>
       </c>
       <c r="P7" s="7" t="s">
         <v>5</v>
@@ -3894,7 +3921,7 @@
         <v>395</v>
       </c>
       <c r="G8" s="30">
-        <f>COUNTIF(C3:C197,5)</f>
+        <f>COUNTIF(C3:C200,5)</f>
         <v>14</v>
       </c>
       <c r="P8" s="7" t="s">
@@ -3924,7 +3951,7 @@
         <v>396</v>
       </c>
       <c r="G9" s="30">
-        <f>COUNTIF(C3:C197,6)</f>
+        <f>COUNTIF(C3:C200,6)</f>
         <v>10</v>
       </c>
       <c r="P9" s="7" t="s">
@@ -3954,7 +3981,7 @@
         <v>397</v>
       </c>
       <c r="G10" s="30">
-        <f>COUNTIF(C3:C197,7)</f>
+        <f>COUNTIF(C3:C200,7)</f>
         <v>15</v>
       </c>
       <c r="P10" s="7" t="s">
@@ -3984,7 +4011,7 @@
         <v>398</v>
       </c>
       <c r="G11" s="30">
-        <f>COUNTIF(C3:C197,8)</f>
+        <f>COUNTIF(C3:C200,8)</f>
         <v>21</v>
       </c>
       <c r="P11" s="7" t="s">
@@ -4014,7 +4041,7 @@
         <v>399</v>
       </c>
       <c r="G12" s="30">
-        <f>COUNTIF(C3:C198,9)</f>
+        <f>COUNTIF(C3:C200,9)</f>
         <v>5</v>
       </c>
       <c r="H12" t="s">
@@ -4022,7 +4049,7 @@
       </c>
       <c r="I12">
         <f>SUM(G3:G12)</f>
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="P12" s="7" t="s">
         <v>10</v>
@@ -6407,17 +6434,14 @@
       </c>
     </row>
     <row r="116" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="B116" s="17" t="s">
-        <v>315</v>
-      </c>
-      <c r="C116" s="18">
-        <v>4</v>
-      </c>
-      <c r="E116" s="2" t="s">
-        <v>406</v>
+      <c r="A116" s="15" t="s">
+        <v>411</v>
+      </c>
+      <c r="B116" s="15" t="s">
+        <v>311</v>
+      </c>
+      <c r="C116" s="16">
+        <v>3</v>
       </c>
       <c r="F116" s="10"/>
       <c r="G116" s="1"/>
@@ -6432,17 +6456,14 @@
       </c>
     </row>
     <row r="117" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="B117" s="17" t="s">
-        <v>311</v>
-      </c>
-      <c r="C117" s="18">
-        <v>4</v>
-      </c>
-      <c r="E117" s="2" t="s">
-        <v>407</v>
+      <c r="A117" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B117" s="15" t="s">
+        <v>321</v>
+      </c>
+      <c r="C117" s="16">
+        <v>3</v>
       </c>
       <c r="F117" s="10"/>
       <c r="G117" s="1"/>
@@ -6457,17 +6478,14 @@
       </c>
     </row>
     <row r="118" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="B118" s="17" t="s">
-        <v>321</v>
-      </c>
-      <c r="C118" s="18">
-        <v>4</v>
-      </c>
-      <c r="E118" s="10" t="s">
-        <v>404</v>
+      <c r="A118" s="15" t="s">
+        <v>412</v>
+      </c>
+      <c r="B118" s="15" t="s">
+        <v>319</v>
+      </c>
+      <c r="C118" s="16">
+        <v>3</v>
       </c>
       <c r="F118" s="10"/>
       <c r="G118" s="1"/>
@@ -6482,17 +6500,14 @@
       </c>
     </row>
     <row r="119" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="B119" s="17" t="s">
-        <v>314</v>
-      </c>
-      <c r="C119" s="18">
-        <v>4</v>
-      </c>
-      <c r="E119" s="10" t="s">
-        <v>405</v>
+      <c r="A119" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B119" s="15" t="s">
+        <v>322</v>
+      </c>
+      <c r="C119" s="16">
+        <v>3</v>
       </c>
       <c r="F119" s="10"/>
       <c r="G119" s="1"/>
@@ -6507,17 +6522,14 @@
       </c>
     </row>
     <row r="120" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="B120" s="17" t="s">
-        <v>319</v>
-      </c>
-      <c r="C120" s="18">
-        <v>4</v>
-      </c>
-      <c r="E120" s="2" t="s">
-        <v>408</v>
+      <c r="A120" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B120" s="15" t="s">
+        <v>317</v>
+      </c>
+      <c r="C120" s="16">
+        <v>3</v>
       </c>
       <c r="F120" s="10"/>
       <c r="G120" s="1"/>
@@ -6532,17 +6544,14 @@
       </c>
     </row>
     <row r="121" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="B121" s="17" t="s">
-        <v>322</v>
-      </c>
-      <c r="C121" s="18">
-        <v>4</v>
-      </c>
-      <c r="E121" s="2" t="s">
-        <v>410</v>
+      <c r="A121" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B121" s="15" t="s">
+        <v>312</v>
+      </c>
+      <c r="C121" s="16">
+        <v>3</v>
       </c>
       <c r="F121" s="10"/>
       <c r="G121" s="1"/>
@@ -6557,14 +6566,14 @@
       </c>
     </row>
     <row r="122" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="B122" s="17" t="s">
-        <v>317</v>
-      </c>
-      <c r="C122" s="18">
-        <v>4</v>
+      <c r="A122" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B122" s="15" t="s">
+        <v>323</v>
+      </c>
+      <c r="C122" s="16">
+        <v>3</v>
       </c>
       <c r="E122" s="10"/>
       <c r="F122" s="10"/>
@@ -6580,18 +6589,15 @@
       </c>
     </row>
     <row r="123" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="17" t="s">
-        <v>121</v>
-      </c>
-      <c r="B123" s="34" t="s">
-        <v>308</v>
-      </c>
-      <c r="C123" s="18">
-        <v>4</v>
-      </c>
-      <c r="E123" s="10"/>
-      <c r="F123" s="10"/>
-      <c r="G123" s="1"/>
+      <c r="A123" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B123" s="15" t="s">
+        <v>318</v>
+      </c>
+      <c r="C123" s="16">
+        <v>3</v>
+      </c>
       <c r="P123" s="17" t="s">
         <v>121</v>
       </c>
@@ -6603,14 +6609,14 @@
       </c>
     </row>
     <row r="124" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="B124" s="17" t="s">
-        <v>312</v>
-      </c>
-      <c r="C124" s="18">
-        <v>4</v>
+      <c r="A124" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B124" s="15" t="s">
+        <v>316</v>
+      </c>
+      <c r="C124" s="16">
+        <v>3</v>
       </c>
       <c r="E124" s="10"/>
       <c r="F124" s="10"/>
@@ -6626,18 +6632,16 @@
       </c>
     </row>
     <row r="125" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="B125" s="17" t="s">
-        <v>323</v>
-      </c>
-      <c r="C125" s="18">
-        <v>4</v>
+      <c r="A125" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B125" s="15" t="s">
+        <v>320</v>
+      </c>
+      <c r="C125" s="16">
+        <v>3</v>
       </c>
       <c r="E125" s="10"/>
-      <c r="F125" s="10"/>
-      <c r="G125" s="1"/>
       <c r="P125" s="17" t="s">
         <v>123</v>
       </c>
@@ -6650,17 +6654,15 @@
     </row>
     <row r="126" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A126" s="17" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B126" s="17" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C126" s="18">
         <v>4</v>
       </c>
       <c r="E126" s="10"/>
-      <c r="F126" s="10"/>
-      <c r="G126" s="1"/>
       <c r="P126" s="17" t="s">
         <v>124</v>
       </c>
@@ -6673,17 +6675,15 @@
     </row>
     <row r="127" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A127" s="17" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B127" s="17" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C127" s="18">
         <v>4</v>
       </c>
       <c r="E127" s="10"/>
-      <c r="F127" s="10"/>
-      <c r="G127" s="1"/>
       <c r="P127" s="17" t="s">
         <v>125</v>
       </c>
@@ -6696,17 +6696,15 @@
     </row>
     <row r="128" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="17" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B128" s="17" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="C128" s="18">
         <v>4</v>
       </c>
       <c r="E128" s="10"/>
-      <c r="F128" s="10"/>
-      <c r="G128" s="1"/>
       <c r="P128" s="17" t="s">
         <v>126</v>
       </c>
@@ -6719,17 +6717,15 @@
     </row>
     <row r="129" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A129" s="17" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B129" s="17" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C129" s="18">
         <v>4</v>
       </c>
       <c r="E129" s="10"/>
-      <c r="F129" s="10"/>
-      <c r="G129" s="1"/>
       <c r="P129" s="17" t="s">
         <v>127</v>
       </c>
@@ -6742,17 +6738,15 @@
     </row>
     <row r="130" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A130" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="B130" s="17" t="s">
-        <v>310</v>
+        <v>129</v>
+      </c>
+      <c r="B130" s="37" t="s">
+        <v>406</v>
       </c>
       <c r="C130" s="18">
         <v>4</v>
       </c>
       <c r="E130" s="10"/>
-      <c r="F130" s="10"/>
-      <c r="G130" s="1"/>
       <c r="P130" s="17" t="s">
         <v>128</v>
       </c>
@@ -6765,17 +6759,15 @@
     </row>
     <row r="131" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A131" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="B131" s="17" t="s">
-        <v>313</v>
+        <v>413</v>
+      </c>
+      <c r="B131" s="37" t="s">
+        <v>407</v>
       </c>
       <c r="C131" s="18">
         <v>4</v>
       </c>
       <c r="E131" s="10"/>
-      <c r="F131" s="10"/>
-      <c r="G131" s="1"/>
       <c r="P131" s="17" t="s">
         <v>129</v>
       </c>
@@ -6787,18 +6779,16 @@
       </c>
     </row>
     <row r="132" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="19" t="s">
-        <v>130</v>
-      </c>
-      <c r="B132" s="19" t="s">
-        <v>326</v>
-      </c>
-      <c r="C132" s="20">
-        <v>5</v>
+      <c r="A132" s="17" t="s">
+        <v>414</v>
+      </c>
+      <c r="B132" s="17" t="s">
+        <v>404</v>
+      </c>
+      <c r="C132" s="18">
+        <v>4</v>
       </c>
       <c r="E132" s="10"/>
-      <c r="F132" s="10"/>
-      <c r="G132" s="1"/>
       <c r="P132" s="19" t="s">
         <v>130</v>
       </c>
@@ -6810,18 +6800,16 @@
       </c>
     </row>
     <row r="133" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="B133" s="19" t="s">
-        <v>328</v>
-      </c>
-      <c r="C133" s="20">
-        <v>5</v>
+      <c r="A133" s="17" t="s">
+        <v>415</v>
+      </c>
+      <c r="B133" s="17" t="s">
+        <v>405</v>
+      </c>
+      <c r="C133" s="18">
+        <v>4</v>
       </c>
       <c r="E133" s="10"/>
-      <c r="F133" s="10"/>
-      <c r="G133" s="1"/>
       <c r="P133" s="19" t="s">
         <v>131</v>
       </c>
@@ -6833,18 +6821,16 @@
       </c>
     </row>
     <row r="134" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="B134" s="19" t="s">
-        <v>332</v>
-      </c>
-      <c r="C134" s="20">
-        <v>5</v>
+      <c r="A134" s="17" t="s">
+        <v>416</v>
+      </c>
+      <c r="B134" s="37" t="s">
+        <v>408</v>
+      </c>
+      <c r="C134" s="18">
+        <v>4</v>
       </c>
       <c r="E134" s="10"/>
-      <c r="F134" s="10"/>
-      <c r="G134" s="1"/>
       <c r="P134" s="19" t="s">
         <v>132</v>
       </c>
@@ -6856,14 +6842,14 @@
       </c>
     </row>
     <row r="135" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="19" t="s">
-        <v>133</v>
-      </c>
-      <c r="B135" s="19" t="s">
-        <v>333</v>
-      </c>
-      <c r="C135" s="20">
-        <v>5</v>
+      <c r="A135" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="B135" s="37" t="s">
+        <v>410</v>
+      </c>
+      <c r="C135" s="18">
+        <v>4</v>
       </c>
       <c r="E135" s="10"/>
       <c r="F135" s="10"/>
@@ -6880,10 +6866,10 @@
     </row>
     <row r="136" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A136" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="B136" s="35" t="s">
-        <v>327</v>
+        <v>130</v>
+      </c>
+      <c r="B136" s="19" t="s">
+        <v>326</v>
       </c>
       <c r="C136" s="20">
         <v>5</v>
@@ -6903,10 +6889,10 @@
     </row>
     <row r="137" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A137" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="B137" s="35" t="s">
-        <v>334</v>
+        <v>131</v>
+      </c>
+      <c r="B137" s="19" t="s">
+        <v>328</v>
       </c>
       <c r="C137" s="20">
         <v>5</v>
@@ -6926,10 +6912,10 @@
     </row>
     <row r="138" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="19" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B138" s="19" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C138" s="20">
         <v>5</v>
@@ -6949,10 +6935,10 @@
     </row>
     <row r="139" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A139" s="19" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B139" s="19" t="s">
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="C139" s="20">
         <v>5</v>
@@ -6972,10 +6958,10 @@
     </row>
     <row r="140" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A140" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="B140" s="19" t="s">
-        <v>324</v>
+        <v>134</v>
+      </c>
+      <c r="B140" s="35" t="s">
+        <v>327</v>
       </c>
       <c r="C140" s="20">
         <v>5</v>
@@ -6995,10 +6981,10 @@
     </row>
     <row r="141" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="B141" s="19" t="s">
-        <v>329</v>
+        <v>135</v>
+      </c>
+      <c r="B141" s="35" t="s">
+        <v>334</v>
       </c>
       <c r="C141" s="20">
         <v>5</v>
@@ -7018,10 +7004,10 @@
     </row>
     <row r="142" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="19" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B142" s="19" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C142" s="20">
         <v>5</v>
@@ -7041,10 +7027,10 @@
     </row>
     <row r="143" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A143" s="19" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B143" s="19" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="C143" s="20">
         <v>5</v>
@@ -7064,10 +7050,10 @@
     </row>
     <row r="144" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A144" s="19" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B144" s="19" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="C144" s="20">
         <v>5</v>
@@ -7087,10 +7073,10 @@
     </row>
     <row r="145" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="19" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B145" s="19" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C145" s="20">
         <v>5</v>
@@ -7109,14 +7095,14 @@
       </c>
     </row>
     <row r="146" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="21" t="s">
-        <v>144</v>
-      </c>
-      <c r="B146" s="21" t="s">
-        <v>338</v>
-      </c>
-      <c r="C146" s="22">
-        <v>6</v>
+      <c r="A146" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B146" s="19" t="s">
+        <v>336</v>
+      </c>
+      <c r="C146" s="20">
+        <v>5</v>
       </c>
       <c r="E146" s="10"/>
       <c r="F146" s="10"/>
@@ -7132,14 +7118,14 @@
       </c>
     </row>
     <row r="147" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="B147" s="21" t="s">
-        <v>340</v>
-      </c>
-      <c r="C147" s="22">
-        <v>6</v>
+      <c r="A147" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="B147" s="19" t="s">
+        <v>337</v>
+      </c>
+      <c r="C147" s="20">
+        <v>5</v>
       </c>
       <c r="E147" s="10"/>
       <c r="F147" s="10"/>
@@ -7155,14 +7141,14 @@
       </c>
     </row>
     <row r="148" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="B148" s="21" t="s">
-        <v>343</v>
-      </c>
-      <c r="C148" s="22">
-        <v>6</v>
+      <c r="A148" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="B148" s="19" t="s">
+        <v>331</v>
+      </c>
+      <c r="C148" s="20">
+        <v>5</v>
       </c>
       <c r="E148" s="10"/>
       <c r="F148" s="10"/>
@@ -7178,14 +7164,14 @@
       </c>
     </row>
     <row r="149" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="B149" s="21" t="s">
-        <v>347</v>
-      </c>
-      <c r="C149" s="22">
-        <v>6</v>
+      <c r="A149" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B149" s="19" t="s">
+        <v>330</v>
+      </c>
+      <c r="C149" s="20">
+        <v>5</v>
       </c>
       <c r="E149" s="10"/>
       <c r="F149" s="10"/>
@@ -7202,10 +7188,10 @@
     </row>
     <row r="150" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A150" s="21" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="B150" s="21" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="C150" s="22">
         <v>6</v>
@@ -7225,10 +7211,10 @@
     </row>
     <row r="151" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A151" s="21" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B151" s="21" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C151" s="22">
         <v>6</v>
@@ -7248,10 +7234,10 @@
     </row>
     <row r="152" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="21" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B152" s="21" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="C152" s="22">
         <v>6</v>
@@ -7271,10 +7257,10 @@
     </row>
     <row r="153" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A153" s="21" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B153" s="21" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="C153" s="22">
         <v>6</v>
@@ -7294,10 +7280,10 @@
     </row>
     <row r="154" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A154" s="21" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B154" s="21" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="C154" s="22">
         <v>6</v>
@@ -7317,10 +7303,10 @@
     </row>
     <row r="155" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A155" s="21" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B155" s="21" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C155" s="22">
         <v>6</v>
@@ -7339,14 +7325,14 @@
       </c>
     </row>
     <row r="156" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="23" t="s">
-        <v>154</v>
-      </c>
-      <c r="B156" s="23" t="s">
-        <v>358</v>
-      </c>
-      <c r="C156" s="24">
-        <v>7</v>
+      <c r="A156" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="B156" s="21" t="s">
+        <v>339</v>
+      </c>
+      <c r="C156" s="22">
+        <v>6</v>
       </c>
       <c r="E156" s="10"/>
       <c r="F156" s="10"/>
@@ -7362,14 +7348,14 @@
       </c>
     </row>
     <row r="157" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="B157" s="23" t="s">
-        <v>356</v>
-      </c>
-      <c r="C157" s="24">
-        <v>7</v>
+      <c r="A157" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="B157" s="21" t="s">
+        <v>344</v>
+      </c>
+      <c r="C157" s="22">
+        <v>6</v>
       </c>
       <c r="E157" s="10"/>
       <c r="F157" s="10"/>
@@ -7385,14 +7371,14 @@
       </c>
     </row>
     <row r="158" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A158" s="23" t="s">
-        <v>156</v>
-      </c>
-      <c r="B158" s="23" t="s">
-        <v>355</v>
-      </c>
-      <c r="C158" s="24">
-        <v>7</v>
+      <c r="A158" s="21" t="s">
+        <v>152</v>
+      </c>
+      <c r="B158" s="21" t="s">
+        <v>345</v>
+      </c>
+      <c r="C158" s="22">
+        <v>6</v>
       </c>
       <c r="E158" s="10"/>
       <c r="F158" s="10"/>
@@ -7408,14 +7394,14 @@
       </c>
     </row>
     <row r="159" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A159" s="23" t="s">
-        <v>157</v>
-      </c>
-      <c r="B159" s="36" t="s">
-        <v>357</v>
-      </c>
-      <c r="C159" s="24">
-        <v>7</v>
+      <c r="A159" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="B159" s="21" t="s">
+        <v>342</v>
+      </c>
+      <c r="C159" s="22">
+        <v>6</v>
       </c>
       <c r="E159" s="10"/>
       <c r="F159" s="10"/>
@@ -7432,10 +7418,10 @@
     </row>
     <row r="160" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A160" s="23" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B160" s="23" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
       <c r="C160" s="24">
         <v>7</v>
@@ -7455,10 +7441,10 @@
     </row>
     <row r="161" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A161" s="23" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B161" s="23" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="C161" s="24">
         <v>7</v>
@@ -7478,10 +7464,10 @@
     </row>
     <row r="162" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A162" s="23" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B162" s="23" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="C162" s="24">
         <v>7</v>
@@ -7501,10 +7487,10 @@
     </row>
     <row r="163" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A163" s="23" t="s">
-        <v>161</v>
-      </c>
-      <c r="B163" s="23" t="s">
-        <v>350</v>
+        <v>157</v>
+      </c>
+      <c r="B163" s="36" t="s">
+        <v>357</v>
       </c>
       <c r="C163" s="24">
         <v>7</v>
@@ -7524,10 +7510,10 @@
     </row>
     <row r="164" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A164" s="23" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B164" s="23" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
       <c r="C164" s="24">
         <v>7</v>
@@ -7547,10 +7533,10 @@
     </row>
     <row r="165" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A165" s="23" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B165" s="23" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="C165" s="24">
         <v>7</v>
@@ -7570,10 +7556,10 @@
     </row>
     <row r="166" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A166" s="23" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B166" s="23" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="C166" s="24">
         <v>7</v>
@@ -7593,10 +7579,10 @@
     </row>
     <row r="167" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A167" s="23" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B167" s="23" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="C167" s="24">
         <v>7</v>
@@ -7616,10 +7602,10 @@
     </row>
     <row r="168" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A168" s="23" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B168" s="23" t="s">
-        <v>351</v>
+        <v>362</v>
       </c>
       <c r="C168" s="24">
         <v>7</v>
@@ -7639,10 +7625,10 @@
     </row>
     <row r="169" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A169" s="23" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="B169" s="23" t="s">
-        <v>349</v>
+        <v>361</v>
       </c>
       <c r="C169" s="24">
         <v>7</v>
@@ -7662,10 +7648,10 @@
     </row>
     <row r="170" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A170" s="23" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B170" s="23" t="s">
-        <v>348</v>
+        <v>360</v>
       </c>
       <c r="C170" s="24">
         <v>7</v>
@@ -7684,14 +7670,14 @@
       </c>
     </row>
     <row r="171" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A171" s="25" t="s">
-        <v>169</v>
-      </c>
-      <c r="B171" s="25" t="s">
-        <v>372</v>
-      </c>
-      <c r="C171" s="26">
-        <v>8</v>
+      <c r="A171" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="B171" s="23" t="s">
+        <v>359</v>
+      </c>
+      <c r="C171" s="24">
+        <v>7</v>
       </c>
       <c r="E171" s="10"/>
       <c r="F171" s="10"/>
@@ -7707,14 +7693,14 @@
       </c>
     </row>
     <row r="172" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A172" s="25" t="s">
-        <v>170</v>
-      </c>
-      <c r="B172" s="25" t="s">
-        <v>371</v>
-      </c>
-      <c r="C172" s="26">
-        <v>8</v>
+      <c r="A172" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="B172" s="23" t="s">
+        <v>351</v>
+      </c>
+      <c r="C172" s="24">
+        <v>7</v>
       </c>
       <c r="E172" s="10"/>
       <c r="F172" s="10"/>
@@ -7730,14 +7716,14 @@
       </c>
     </row>
     <row r="173" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A173" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="B173" s="25" t="s">
-        <v>370</v>
-      </c>
-      <c r="C173" s="26">
-        <v>8</v>
+      <c r="A173" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="B173" s="23" t="s">
+        <v>349</v>
+      </c>
+      <c r="C173" s="24">
+        <v>7</v>
       </c>
       <c r="E173" s="10"/>
       <c r="F173" s="10"/>
@@ -7753,14 +7739,14 @@
       </c>
     </row>
     <row r="174" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A174" s="25" t="s">
-        <v>172</v>
-      </c>
-      <c r="B174" s="25" t="s">
-        <v>366</v>
-      </c>
-      <c r="C174" s="26">
-        <v>8</v>
+      <c r="A174" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="B174" s="23" t="s">
+        <v>348</v>
+      </c>
+      <c r="C174" s="24">
+        <v>7</v>
       </c>
       <c r="E174" s="10"/>
       <c r="F174" s="10"/>
@@ -7777,10 +7763,10 @@
     </row>
     <row r="175" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A175" s="25" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B175" s="25" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C175" s="26">
         <v>8</v>
@@ -7800,10 +7786,10 @@
     </row>
     <row r="176" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="25" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B176" s="25" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="C176" s="26">
         <v>8</v>
@@ -7823,10 +7809,10 @@
     </row>
     <row r="177" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A177" s="25" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="B177" s="25" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="C177" s="26">
         <v>8</v>
@@ -7846,10 +7832,10 @@
     </row>
     <row r="178" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A178" s="25" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B178" s="25" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C178" s="26">
         <v>8</v>
@@ -7869,10 +7855,10 @@
     </row>
     <row r="179" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A179" s="25" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B179" s="25" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C179" s="26">
         <v>8</v>
@@ -7892,10 +7878,10 @@
     </row>
     <row r="180" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A180" s="25" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B180" s="25" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="C180" s="26">
         <v>8</v>
@@ -7915,10 +7901,10 @@
     </row>
     <row r="181" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A181" s="25" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="B181" s="25" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="C181" s="26">
         <v>8</v>
@@ -7938,10 +7924,10 @@
     </row>
     <row r="182" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A182" s="25" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B182" s="25" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="C182" s="26">
         <v>8</v>
@@ -7961,10 +7947,10 @@
     </row>
     <row r="183" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A183" s="25" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B183" s="25" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="C183" s="26">
         <v>8</v>
@@ -7984,10 +7970,10 @@
     </row>
     <row r="184" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A184" s="25" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="B184" s="25" t="s">
-        <v>380</v>
+        <v>367</v>
       </c>
       <c r="C184" s="26">
         <v>8</v>
@@ -8007,10 +7993,10 @@
     </row>
     <row r="185" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="25" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B185" s="25" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
       <c r="C185" s="26">
         <v>8</v>
@@ -8030,10 +8016,10 @@
     </row>
     <row r="186" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="25" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B186" s="25" t="s">
-        <v>381</v>
+        <v>369</v>
       </c>
       <c r="C186" s="26">
         <v>8</v>
@@ -8053,10 +8039,10 @@
     </row>
     <row r="187" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A187" s="25" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="B187" s="25" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="C187" s="26">
         <v>8</v>
@@ -8076,10 +8062,10 @@
     </row>
     <row r="188" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A188" s="25" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B188" s="25" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="C188" s="26">
         <v>8</v>
@@ -8099,10 +8085,10 @@
     </row>
     <row r="189" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="25" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="B189" s="25" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C189" s="26">
         <v>8</v>
@@ -8122,10 +8108,10 @@
     </row>
     <row r="190" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A190" s="25" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B190" s="25" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C190" s="26">
         <v>8</v>
@@ -8145,10 +8131,10 @@
     </row>
     <row r="191" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A191" s="25" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B191" s="25" t="s">
-        <v>364</v>
+        <v>376</v>
       </c>
       <c r="C191" s="26">
         <v>8</v>
@@ -8167,14 +8153,14 @@
       </c>
     </row>
     <row r="192" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A192" s="27" t="s">
-        <v>190</v>
-      </c>
-      <c r="B192" s="27" t="s">
-        <v>387</v>
-      </c>
-      <c r="C192" s="28">
-        <v>9</v>
+      <c r="A192" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="B192" s="25" t="s">
+        <v>378</v>
+      </c>
+      <c r="C192" s="26">
+        <v>8</v>
       </c>
       <c r="E192" s="10"/>
       <c r="F192" s="10"/>
@@ -8190,14 +8176,14 @@
       </c>
     </row>
     <row r="193" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A193" s="27" t="s">
-        <v>191</v>
-      </c>
-      <c r="B193" s="27" t="s">
-        <v>385</v>
-      </c>
-      <c r="C193" s="28">
-        <v>9</v>
+      <c r="A193" s="25" t="s">
+        <v>187</v>
+      </c>
+      <c r="B193" s="25" t="s">
+        <v>377</v>
+      </c>
+      <c r="C193" s="26">
+        <v>8</v>
       </c>
       <c r="E193" s="10"/>
       <c r="F193" s="10"/>
@@ -8213,14 +8199,14 @@
       </c>
     </row>
     <row r="194" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A194" s="27" t="s">
-        <v>192</v>
-      </c>
-      <c r="B194" s="27" t="s">
-        <v>386</v>
-      </c>
-      <c r="C194" s="28">
-        <v>9</v>
+      <c r="A194" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="B194" s="25" t="s">
+        <v>382</v>
+      </c>
+      <c r="C194" s="26">
+        <v>8</v>
       </c>
       <c r="E194" s="10"/>
       <c r="F194" s="10"/>
@@ -8236,14 +8222,14 @@
       </c>
     </row>
     <row r="195" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A195" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="B195" s="27" t="s">
-        <v>384</v>
-      </c>
-      <c r="C195" s="28">
-        <v>9</v>
+      <c r="A195" s="25" t="s">
+        <v>189</v>
+      </c>
+      <c r="B195" s="25" t="s">
+        <v>364</v>
+      </c>
+      <c r="C195" s="26">
+        <v>8</v>
       </c>
       <c r="E195" s="10"/>
       <c r="F195" s="10"/>
@@ -8260,10 +8246,10 @@
     </row>
     <row r="196" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A196" s="27" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B196" s="27" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C196" s="28">
         <v>9</v>
@@ -8281,10 +8267,55 @@
         <v>9</v>
       </c>
     </row>
+    <row r="197" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A197" s="27" t="s">
+        <v>191</v>
+      </c>
+      <c r="B197" s="27" t="s">
+        <v>385</v>
+      </c>
+      <c r="C197" s="28">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="198" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A198" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="B198" s="27" t="s">
+        <v>386</v>
+      </c>
+      <c r="C198" s="28">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="199" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A199" s="27" t="s">
+        <v>193</v>
+      </c>
+      <c r="B199" s="27" t="s">
+        <v>384</v>
+      </c>
+      <c r="C199" s="28">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="200" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A200" s="27" t="s">
+        <v>194</v>
+      </c>
+      <c r="B200" s="27" t="s">
+        <v>388</v>
+      </c>
+      <c r="C200" s="28">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B146:B155">
-    <sortCondition ref="B146:B155"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B150:B159">
+    <sortCondition ref="B150:B159"/>
   </sortState>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>